<commit_message>
[ADD] Test de integracion a las rutas escuela
</commit_message>
<xml_diff>
--- a/Codigos de errores.xlsx
+++ b/Codigos de errores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Desktop\EscuelasProject\escuelas_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A9E0680-B501-4493-9156-973F72B39E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A65115-654B-45B6-B57E-AAD6BF9D5947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{08DD28E9-37C6-4B48-9B2E-65347E2FB0A6}"/>
+    <workbookView xWindow="20370" yWindow="-525" windowWidth="20640" windowHeight="11310" xr2:uid="{08DD28E9-37C6-4B48-9B2E-65347E2FB0A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Error de validacion del dto</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Entidad ya existente en base de datos</t>
+  </si>
+  <si>
+    <t>Argumentos de ruta invalidos</t>
+  </si>
+  <si>
+    <t>Ruta de api invalida</t>
+  </si>
+  <si>
+    <t>server internal error</t>
   </si>
 </sst>
 </file>
@@ -400,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208D006B-3CDE-4518-95DA-E4AF72A6ADC7}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,15 +420,18 @@
     <col min="2" max="2" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -427,28 +439,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>